<commit_message>
Bot 100% finalizado e sem bugs
</commit_message>
<xml_diff>
--- a/Contatos2S.xlsx
+++ b/Contatos2S.xlsx
@@ -1,34 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunatoledo/Documents/Visual-Studio-Code/WebEx-Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221BEC42-3E6E-3D47-AB58-DCA21238FB38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43759C2B-CF52-2F43-804E-B64EB5BD91D5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="460" windowWidth="21100" windowHeight="16080" xr2:uid="{75483642-E0BB-40D6-AD7E-FAAB2DA70647}"/>
+    <workbookView xWindow="2960" yWindow="460" windowWidth="21100" windowHeight="16080" xr2:uid="{75483642-E0BB-40D6-AD7E-FAAB2DA70647}"/>
   </bookViews>
   <sheets>
-    <sheet name="Contato" sheetId="1" r:id="rId1"/>
+    <sheet name="Contato_2S" sheetId="1" r:id="rId1"/>
+    <sheet name="Contato_Cisco" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contato!$A$1:$F$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contato_2S!$A$1:$F$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contato_Cisco!$A$1:$D$79</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="549">
   <si>
     <t>adriana.fulaz@2s.com.br</t>
   </si>
@@ -183,9 +190,6 @@
     <t>jose.pereira@2s.com.br</t>
   </si>
   <si>
-    <t>julia.souza@2s.com.br</t>
-  </si>
-  <si>
     <t>juliana.cunha@2s.com.br</t>
   </si>
   <si>
@@ -474,9 +478,6 @@
     <t>Jose Pereira</t>
   </si>
   <si>
-    <t>Julia Souza</t>
-  </si>
-  <si>
     <t>Juliana Cunha</t>
   </si>
   <si>
@@ -757,13 +758,937 @@
   </si>
   <si>
     <t xml:space="preserve">Não consta </t>
+  </si>
+  <si>
+    <t>Benny Zatyrko</t>
+  </si>
+  <si>
+    <t>Homero Ribeiro</t>
+  </si>
+  <si>
+    <t>João Sardinha</t>
+  </si>
+  <si>
+    <t>Jose Alfredo</t>
+  </si>
+  <si>
+    <t>Lenizi Nardomarino</t>
+  </si>
+  <si>
+    <t>bzatyrko@cisco.com</t>
+  </si>
+  <si>
+    <t>jsardinh@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 5508-9969</t>
+  </si>
+  <si>
+    <t>(11) 99251-9829</t>
+  </si>
+  <si>
+    <t>(11) 99250-0037</t>
+  </si>
+  <si>
+    <t>(11) 5502-3195</t>
+  </si>
+  <si>
+    <t>Marcelo Ehalt</t>
+  </si>
+  <si>
+    <t>Severiano Macedo</t>
+  </si>
+  <si>
+    <t>Marco Sena</t>
+  </si>
+  <si>
+    <t>Laércio Albuquerque</t>
+  </si>
+  <si>
+    <t>Fabio Peake</t>
+  </si>
+  <si>
+    <t>hribeiro@cisco.com</t>
+  </si>
+  <si>
+    <t>josalfre@cisco.com</t>
+  </si>
+  <si>
+    <t>lnardoma@cisco.com</t>
+  </si>
+  <si>
+    <t>mehalt@cisco.com</t>
+  </si>
+  <si>
+    <t>smacedoj@cisco.com</t>
+  </si>
+  <si>
+    <t>msena@cisco.com</t>
+  </si>
+  <si>
+    <t>lalbuque@cisco.com</t>
+  </si>
+  <si>
+    <t>fapeake@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 5508-1553</t>
+  </si>
+  <si>
+    <t>(11) 99251-9881</t>
+  </si>
+  <si>
+    <t>(11) 5508-9954</t>
+  </si>
+  <si>
+    <t>(11) 99266-6333</t>
+  </si>
+  <si>
+    <t>(11) 99249-1143</t>
+  </si>
+  <si>
+    <t>(11) 5508-1524</t>
+  </si>
+  <si>
+    <t>(11) 96411-6285</t>
+  </si>
+  <si>
+    <t>Adriano Andreoli</t>
+  </si>
+  <si>
+    <t>Felipe Pratellesi</t>
+  </si>
+  <si>
+    <t>Marcelo Silva</t>
+  </si>
+  <si>
+    <t>Aryane Mincovschi</t>
+  </si>
+  <si>
+    <t>Daniel Albuquerque</t>
+  </si>
+  <si>
+    <t>Rodolfo Cunha</t>
+  </si>
+  <si>
+    <t>Carolina Barnabé</t>
+  </si>
+  <si>
+    <t>Rafael Penna</t>
+  </si>
+  <si>
+    <t>Bruna Gabech</t>
+  </si>
+  <si>
+    <t>Emerson Yoshimura</t>
+  </si>
+  <si>
+    <t>Felipe Cecchi</t>
+  </si>
+  <si>
+    <t>Felipe Teles</t>
+  </si>
+  <si>
+    <t>Fernando Silva</t>
+  </si>
+  <si>
+    <t>Flavio Portes</t>
+  </si>
+  <si>
+    <t>Gabriela Giovanni</t>
+  </si>
+  <si>
+    <t>Guilherme Araújo</t>
+  </si>
+  <si>
+    <t>Leandro Scaranello</t>
+  </si>
+  <si>
+    <t>Marcio Biltoveni</t>
+  </si>
+  <si>
+    <t>Paula Muto</t>
+  </si>
+  <si>
+    <t>Rafael Farias</t>
+  </si>
+  <si>
+    <t>Renata Nascimento</t>
+  </si>
+  <si>
+    <t>Rita Magno</t>
+  </si>
+  <si>
+    <t>Claudia Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniela Roque </t>
+  </si>
+  <si>
+    <t>Danilo Andrade</t>
+  </si>
+  <si>
+    <t>Eduardo Frade</t>
+  </si>
+  <si>
+    <t>Fabiano Prado</t>
+  </si>
+  <si>
+    <t>Luiz Cristovao</t>
+  </si>
+  <si>
+    <t>Soraya Lima Thorsjo</t>
+  </si>
+  <si>
+    <t>Yuri Yaksic</t>
+  </si>
+  <si>
+    <t>Mauro Levin</t>
+  </si>
+  <si>
+    <t>Andre Gurgel</t>
+  </si>
+  <si>
+    <t>Edson Machado</t>
+  </si>
+  <si>
+    <t>Eduardo Abud</t>
+  </si>
+  <si>
+    <t>Eduardo Yamauchi</t>
+  </si>
+  <si>
+    <t>Pedro Ascenção</t>
+  </si>
+  <si>
+    <t>Andrey Cassemiro</t>
+  </si>
+  <si>
+    <t>Daniel Brochado</t>
+  </si>
+  <si>
+    <t>Edson Barbosa</t>
+  </si>
+  <si>
+    <t>Eliane Gasparotto</t>
+  </si>
+  <si>
+    <t>Fabiano Furlan</t>
+  </si>
+  <si>
+    <t>Felipe Amorim</t>
+  </si>
+  <si>
+    <t>Felipe Mellado</t>
+  </si>
+  <si>
+    <t>Flavio Correa</t>
+  </si>
+  <si>
+    <t>Jocelyn Lima Neto</t>
+  </si>
+  <si>
+    <t>Kazuo Yamamoto</t>
+  </si>
+  <si>
+    <t>Maurício Ribeiro</t>
+  </si>
+  <si>
+    <t>Ricardo Mesquita</t>
+  </si>
+  <si>
+    <t>Ricardo Vallino</t>
+  </si>
+  <si>
+    <t>Rodrigo Rezende</t>
+  </si>
+  <si>
+    <t>Rosemary Arakaki</t>
+  </si>
+  <si>
+    <t>Sergio Polizer</t>
+  </si>
+  <si>
+    <t>Tais Ferreira</t>
+  </si>
+  <si>
+    <t>Vinicius Golin</t>
+  </si>
+  <si>
+    <t>Vinicius Pereira</t>
+  </si>
+  <si>
+    <t>Rafael Guerra</t>
+  </si>
+  <si>
+    <t>Antonio Ximenes</t>
+  </si>
+  <si>
+    <t>Ricardo Pedras</t>
+  </si>
+  <si>
+    <t>Luiz Braga</t>
+  </si>
+  <si>
+    <t>Ricardo Ogata</t>
+  </si>
+  <si>
+    <t>Daniela Subhia</t>
+  </si>
+  <si>
+    <t>Vinicius Gruppi</t>
+  </si>
+  <si>
+    <t>Antonio Machado</t>
+  </si>
+  <si>
+    <t>aandreol@cisco.com</t>
+  </si>
+  <si>
+    <t>fpratell@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 97181-8270</t>
+  </si>
+  <si>
+    <t>(11) 98473-9416</t>
+  </si>
+  <si>
+    <t>(11) 5508-9989</t>
+  </si>
+  <si>
+    <t>(11) 5508-1591</t>
+  </si>
+  <si>
+    <t>amincovs@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 2666-9091</t>
+  </si>
+  <si>
+    <t>(11) 99408-4310</t>
+  </si>
+  <si>
+    <t>antmacha@cisco.com</t>
+  </si>
+  <si>
+    <t>marcelsi@cisco.com</t>
+  </si>
+  <si>
+    <t>dalbuque@cisco.com</t>
+  </si>
+  <si>
+    <t>rocunha@cisco.com</t>
+  </si>
+  <si>
+    <t>cbarnabe@cisco.com</t>
+  </si>
+  <si>
+    <t>rapenna@cisco.com</t>
+  </si>
+  <si>
+    <t>bgabech@cisco.com</t>
+  </si>
+  <si>
+    <t>eyoshimu@cisco.com</t>
+  </si>
+  <si>
+    <t>fececchi@cisco.com</t>
+  </si>
+  <si>
+    <t>felisilv@cisco.com</t>
+  </si>
+  <si>
+    <t>fernsilv@cisco.com</t>
+  </si>
+  <si>
+    <t>fportes@cisco.com</t>
+  </si>
+  <si>
+    <t>ggiovann@cisco.com</t>
+  </si>
+  <si>
+    <t>leascara@cisco.com</t>
+  </si>
+  <si>
+    <t>mbiltove@cisco.com</t>
+  </si>
+  <si>
+    <t>pamuto@cisco.com</t>
+  </si>
+  <si>
+    <t>rfariasd@cisco.com</t>
+  </si>
+  <si>
+    <t>renascim@cisco.com</t>
+  </si>
+  <si>
+    <t>rimagno@cisco.com</t>
+  </si>
+  <si>
+    <t>clcruz@cisco.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">droque@cisco.com </t>
+  </si>
+  <si>
+    <t>daandrad@cisco.com</t>
+  </si>
+  <si>
+    <t>efrade@cisco.com</t>
+  </si>
+  <si>
+    <t>Eduardo Ritter</t>
+  </si>
+  <si>
+    <t>Kathia Espinosa</t>
+  </si>
+  <si>
+    <t>Fernando Zolko</t>
+  </si>
+  <si>
+    <t>(31) 99943-6315</t>
+  </si>
+  <si>
+    <t>(11) 94287-4718</t>
+  </si>
+  <si>
+    <t>edritter@cisco.com</t>
+  </si>
+  <si>
+    <t>faprado@cisco.com</t>
+  </si>
+  <si>
+    <t>fzolko@cisco.com</t>
+  </si>
+  <si>
+    <t>kespinos@cisco.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcristov@cisco.com </t>
+  </si>
+  <si>
+    <t>nagomes@cisco.com</t>
+  </si>
+  <si>
+    <t>Nathalia Gomes</t>
+  </si>
+  <si>
+    <t>slimasil@cisco.com</t>
+  </si>
+  <si>
+    <t>yyaksic@cisco.com</t>
+  </si>
+  <si>
+    <t>maulevin@cisco.com</t>
+  </si>
+  <si>
+    <t>angurgel@cisco.com</t>
+  </si>
+  <si>
+    <t>emachado@cisco.com</t>
+  </si>
+  <si>
+    <t>eemiliob@cisco.com</t>
+  </si>
+  <si>
+    <t>eyamauch@cisco.com</t>
+  </si>
+  <si>
+    <t>pascenca@cisco.com</t>
+  </si>
+  <si>
+    <t>acassemi@cisco.com</t>
+  </si>
+  <si>
+    <t>dbrochad@cisco.com</t>
+  </si>
+  <si>
+    <t>edbarbos@cisco.com</t>
+  </si>
+  <si>
+    <t>lgasparo@cisco.com</t>
+  </si>
+  <si>
+    <t>ffurlan@cisco.com</t>
+  </si>
+  <si>
+    <t>feamorim@cisco.com</t>
+  </si>
+  <si>
+    <t>femellad@cisco.com</t>
+  </si>
+  <si>
+    <t>flcorrea@cisco.com</t>
+  </si>
+  <si>
+    <t>jlimanet@cisco.com</t>
+  </si>
+  <si>
+    <t>kazyamam@cisco.com</t>
+  </si>
+  <si>
+    <t>mauribei@cisco.com</t>
+  </si>
+  <si>
+    <t>rmesquit@cisco.com</t>
+  </si>
+  <si>
+    <t>rivallin@cisco.com</t>
+  </si>
+  <si>
+    <t>rorezend@cisco.com</t>
+  </si>
+  <si>
+    <t>rarakaki@cisco.com</t>
+  </si>
+  <si>
+    <t>spolizer@cisco.com</t>
+  </si>
+  <si>
+    <t>taferrei@cisco.com</t>
+  </si>
+  <si>
+    <t>vgolin@cisco.com</t>
+  </si>
+  <si>
+    <t>vipereir@cisco.com</t>
+  </si>
+  <si>
+    <t>vtafarel@cisco.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raguerra@cisco.com </t>
+  </si>
+  <si>
+    <t>aximenes@cisco.com</t>
+  </si>
+  <si>
+    <t>rpedras@cisco.com</t>
+  </si>
+  <si>
+    <t>lbragama@cisco.com</t>
+  </si>
+  <si>
+    <t>rogata@cisco.com</t>
+  </si>
+  <si>
+    <t>dsubhia@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 5508-6313</t>
+  </si>
+  <si>
+    <t>(11) 99251-3741</t>
+  </si>
+  <si>
+    <t>Luciano Correa</t>
+  </si>
+  <si>
+    <t>lucorrea@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 5508-2461</t>
+  </si>
+  <si>
+    <t>(11) 5508-9973</t>
+  </si>
+  <si>
+    <t>(11) 5508-2442</t>
+  </si>
+  <si>
+    <t>(11) 99345-8114</t>
+  </si>
+  <si>
+    <t>(11) 95500-0675</t>
+  </si>
+  <si>
+    <t>(11) 5502-3132</t>
+  </si>
+  <si>
+    <t>(11) 99345-4278</t>
+  </si>
+  <si>
+    <t>(11) 99480-5961</t>
+  </si>
+  <si>
+    <t>(11) 99251-9092</t>
+  </si>
+  <si>
+    <t>(11) 5508-2487</t>
+  </si>
+  <si>
+    <t>(11) 99251-6511</t>
+  </si>
+  <si>
+    <t>(11) 5508-1529</t>
+  </si>
+  <si>
+    <t>(11) 99251-5162</t>
+  </si>
+  <si>
+    <t>(11) 99328-0850</t>
+  </si>
+  <si>
+    <t>(11) 5508-2409</t>
+  </si>
+  <si>
+    <t>(11) 94188-6059</t>
+  </si>
+  <si>
+    <t>(11) 5508-2424</t>
+  </si>
+  <si>
+    <t>(11) 5508-2473</t>
+  </si>
+  <si>
+    <t>(11) 99345-0080</t>
+  </si>
+  <si>
+    <t>guaraujo@cisco.com</t>
+  </si>
+  <si>
+    <t>(11) 99251-1124</t>
+  </si>
+  <si>
+    <t>(11) 5508-1551</t>
+  </si>
+  <si>
+    <t>(11) 99251-2474</t>
+  </si>
+  <si>
+    <t>(11) 5508-2496</t>
+  </si>
+  <si>
+    <t>(11) 2666-9118</t>
+  </si>
+  <si>
+    <t>(11) 5508-6318</t>
+  </si>
+  <si>
+    <t>(11) 5508-6334</t>
+  </si>
+  <si>
+    <t>(11) 5508-9968</t>
+  </si>
+  <si>
+    <t>(11) 5502-3120</t>
+  </si>
+  <si>
+    <t>(11) 5502-3111</t>
+  </si>
+  <si>
+    <t>(11) 5508-2434</t>
+  </si>
+  <si>
+    <t>(21) 2483-6353</t>
+  </si>
+  <si>
+    <t>(21) 2483-7275</t>
+  </si>
+  <si>
+    <t>(11) 2666-9111</t>
+  </si>
+  <si>
+    <t>(11) 5502-3196</t>
+  </si>
+  <si>
+    <t>(11) 5508-2489</t>
+  </si>
+  <si>
+    <t>(11) 5508-1534</t>
+  </si>
+  <si>
+    <t>(11) 5502-3138</t>
+  </si>
+  <si>
+    <t>(11) 5508-1584</t>
+  </si>
+  <si>
+    <t>(11) 5508-1562</t>
+  </si>
+  <si>
+    <t>(11) 2666-9248</t>
+  </si>
+  <si>
+    <t>(11) 2666-9148</t>
+  </si>
+  <si>
+    <t>(21) 7629-9426</t>
+  </si>
+  <si>
+    <t>(11) 5502-3113</t>
+  </si>
+  <si>
+    <t>(11) 5508-9907</t>
+  </si>
+  <si>
+    <t>(11) 5508-1576</t>
+  </si>
+  <si>
+    <t>(21) 2483-6310</t>
+  </si>
+  <si>
+    <t>(11) 5502-3178</t>
+  </si>
+  <si>
+    <t>(11) 5508-1589</t>
+  </si>
+  <si>
+    <t>(11) 5502-3122</t>
+  </si>
+  <si>
+    <t>(11) 5508-1579</t>
+  </si>
+  <si>
+    <t>(11) 5502-3197</t>
+  </si>
+  <si>
+    <t>(11) 5508-9922</t>
+  </si>
+  <si>
+    <t>(11) 5508-9906</t>
+  </si>
+  <si>
+    <t>(11) 5508-6329</t>
+  </si>
+  <si>
+    <t>(11) 5508-6338</t>
+  </si>
+  <si>
+    <t>(21) 2483-6308</t>
+  </si>
+  <si>
+    <t>(11) 5508-9986</t>
+  </si>
+  <si>
+    <t>(21) 2483-6390</t>
+  </si>
+  <si>
+    <t>(11) 5508-9995</t>
+  </si>
+  <si>
+    <t>(11) 2666-9316</t>
+  </si>
+  <si>
+    <t>(11) 5508-2469</t>
+  </si>
+  <si>
+    <t>(11) 5508-2412</t>
+  </si>
+  <si>
+    <t>(11) 5508-6312</t>
+  </si>
+  <si>
+    <t>(11) 5508-2456</t>
+  </si>
+  <si>
+    <t>(11) 2666-9293</t>
+  </si>
+  <si>
+    <t>(11) 5508-2420</t>
+  </si>
+  <si>
+    <t>(11) 5508-9928</t>
+  </si>
+  <si>
+    <t>(11) 5508-6316</t>
+  </si>
+  <si>
+    <t>(11) 5502-3193</t>
+  </si>
+  <si>
+    <t>(11) 5508-2495</t>
+  </si>
+  <si>
+    <t>(11) 5508-1570</t>
+  </si>
+  <si>
+    <t>(11) 5508-2457</t>
+  </si>
+  <si>
+    <t>(11) 5508-6345</t>
+  </si>
+  <si>
+    <t>(11) 5502-3184</t>
+  </si>
+  <si>
+    <t>(11) 5508-9924</t>
+  </si>
+  <si>
+    <t>(11) 5508-6337</t>
+  </si>
+  <si>
+    <t>(11) 5502-3166</t>
+  </si>
+  <si>
+    <t>(11) 97634-5431</t>
+  </si>
+  <si>
+    <t>(11) 99251-3297</t>
+  </si>
+  <si>
+    <t>(11) 99260-5331</t>
+  </si>
+  <si>
+    <t>(11) 99230-5378</t>
+  </si>
+  <si>
+    <t>(11) 99251-3510</t>
+  </si>
+  <si>
+    <t>(11) 94287-4780</t>
+  </si>
+  <si>
+    <t>(11) 99251-3124</t>
+  </si>
+  <si>
+    <t>(11) 99251-6750</t>
+  </si>
+  <si>
+    <t>(11) 99250-5937</t>
+  </si>
+  <si>
+    <t>(11) 9251-4718</t>
+  </si>
+  <si>
+    <t>(11) 99251-7614</t>
+  </si>
+  <si>
+    <t>(11) 99250-7147</t>
+  </si>
+  <si>
+    <t>(11) 97659-4093</t>
+  </si>
+  <si>
+    <t>(11) 94134-0606</t>
+  </si>
+  <si>
+    <t>(11) 99251-1236</t>
+  </si>
+  <si>
+    <t>(11) 98233-0042</t>
+  </si>
+  <si>
+    <t>(11) 99251-1472</t>
+  </si>
+  <si>
+    <t>1 408-895-3828</t>
+  </si>
+  <si>
+    <t>1 408-309-4054</t>
+  </si>
+  <si>
+    <t>(11) 99134-1196</t>
+  </si>
+  <si>
+    <t>(11) 99251-5791</t>
+  </si>
+  <si>
+    <t>(11) 99251-6785</t>
+  </si>
+  <si>
+    <t>(21) 98604-7649</t>
+  </si>
+  <si>
+    <t>(11) 99251-8520</t>
+  </si>
+  <si>
+    <t>(21) 7629-5643</t>
+  </si>
+  <si>
+    <t>(11) 99251-5244</t>
+  </si>
+  <si>
+    <t>(11) 99251-3808</t>
+  </si>
+  <si>
+    <t>(11) 99251-9412</t>
+  </si>
+  <si>
+    <t>(11) 95038-1278</t>
+  </si>
+  <si>
+    <t>(11) 99252-9912</t>
+  </si>
+  <si>
+    <t>(11) 99252-3426</t>
+  </si>
+  <si>
+    <t>(11) 99254-0090</t>
+  </si>
+  <si>
+    <t>(11) 99251-9456</t>
+  </si>
+  <si>
+    <t>(11) 99251-7465</t>
+  </si>
+  <si>
+    <t>(11) 98473-9423</t>
+  </si>
+  <si>
+    <t>(11) 99251-2191</t>
+  </si>
+  <si>
+    <t>(11) 99251-8527</t>
+  </si>
+  <si>
+    <t>(11) 99251-5533</t>
+  </si>
+  <si>
+    <t>(21) 97629-5502</t>
+  </si>
+  <si>
+    <t>(11) 99251-7967</t>
+  </si>
+  <si>
+    <t>(11) 97690-6708</t>
+  </si>
+  <si>
+    <t>(11) 99345-2210</t>
+  </si>
+  <si>
+    <t>(11) 99251-5701</t>
+  </si>
+  <si>
+    <t>(61) 99644-1759</t>
+  </si>
+  <si>
+    <t>(11) 96176-5969</t>
+  </si>
+  <si>
+    <t>(51) 99761-8484</t>
+  </si>
+  <si>
+    <t>(11) 99251-7612</t>
+  </si>
+  <si>
+    <t>(11) 98140-5000</t>
+  </si>
+  <si>
+    <t>(11) 99251-1276</t>
+  </si>
+  <si>
+    <t>(11) 97390-9573</t>
+  </si>
+  <si>
+    <t>(11) 99951-8096</t>
+  </si>
+  <si>
+    <t>(11) 9251-9848</t>
+  </si>
+  <si>
+    <t>(21) 97629-5713</t>
+  </si>
+  <si>
+    <t>(11) 96855-3129</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,6 +1708,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -823,11 +1762,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -836,12 +1776,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1172,17 +2138,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF3DC6F-0EC3-4F06-8F1F-DECEF45B43B5}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="167" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
@@ -1190,1415 +2156,2650 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1213</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1229</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1219</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>1291</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1287</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1223</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>1236</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>1248</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>1267</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>1243</v>
       </c>
       <c r="D11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>1218</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>1277</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>1216</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>1263</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>1279</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>1265</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>1245</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>1264</v>
       </c>
       <c r="D19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>1206</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>1234</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>1242</v>
       </c>
       <c r="D22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23">
+        <v>95</v>
+      </c>
+      <c r="C23" s="4">
         <v>1283</v>
       </c>
       <c r="D23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>1210</v>
       </c>
       <c r="D24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>1212</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>1240</v>
       </c>
       <c r="D26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>1295</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>1226</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>1238</v>
       </c>
       <c r="D29" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="4">
         <v>1259</v>
       </c>
       <c r="D30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4">
         <v>1313</v>
       </c>
       <c r="D31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4">
         <v>1270</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="4">
         <v>1227</v>
       </c>
       <c r="D33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="4">
         <v>1260</v>
       </c>
       <c r="D34" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="4">
         <v>1282</v>
       </c>
       <c r="D35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>1314</v>
       </c>
       <c r="D36" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="4">
         <v>1271</v>
       </c>
       <c r="D37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="4">
         <v>1211</v>
       </c>
       <c r="D38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="4">
         <v>1233</v>
       </c>
       <c r="D39" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="4">
         <v>1278</v>
       </c>
       <c r="D40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="4">
         <v>1209</v>
       </c>
       <c r="D41" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="4">
         <v>1205</v>
       </c>
       <c r="D42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43">
+        <v>97</v>
+      </c>
+      <c r="C43" s="4">
         <v>1244</v>
       </c>
       <c r="D43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="4">
         <v>1273</v>
       </c>
       <c r="D44" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="4">
         <v>1215</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="4">
         <v>1214</v>
       </c>
       <c r="D46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
         <v>44</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="4">
         <v>1201</v>
       </c>
       <c r="D47" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="4">
         <v>1217</v>
       </c>
       <c r="D48" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="4">
         <v>1208</v>
       </c>
       <c r="D49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
         <v>47</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="4">
         <v>1231</v>
       </c>
       <c r="D50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>48</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="4">
         <v>1285</v>
       </c>
       <c r="D51" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52">
+        <v>69</v>
+      </c>
+      <c r="C52" s="4">
         <v>1249</v>
       </c>
       <c r="D52" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
         <v>49</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="4">
         <v>1247</v>
       </c>
       <c r="D53" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="4">
         <v>1252</v>
       </c>
       <c r="D54" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
       </c>
-      <c r="C55">
-        <v>1268</v>
+      <c r="C55" s="4">
+        <v>1237</v>
       </c>
       <c r="D55" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56">
-        <v>1237</v>
+        <v>193</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1239</v>
       </c>
       <c r="D56" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>195</v>
-      </c>
-      <c r="C57">
-        <v>1239</v>
+        <v>52</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1241</v>
       </c>
       <c r="D57" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
         <v>53</v>
       </c>
-      <c r="C58">
-        <v>1241</v>
+      <c r="C58" s="4">
+        <v>1269</v>
       </c>
       <c r="D58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
         <v>54</v>
       </c>
-      <c r="C59">
-        <v>1269</v>
+      <c r="C59" s="4">
+        <v>1232</v>
       </c>
       <c r="D59" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
         <v>55</v>
       </c>
-      <c r="C60">
-        <v>1232</v>
+      <c r="C60" s="4">
+        <v>1230</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61">
-        <v>1230</v>
+        <v>194</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1275</v>
       </c>
       <c r="D61" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>196</v>
-      </c>
-      <c r="C62">
-        <v>1275</v>
+        <v>56</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1284</v>
       </c>
       <c r="D62" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
         <v>57</v>
       </c>
-      <c r="C63">
-        <v>1284</v>
+      <c r="C63" s="4">
+        <v>1315</v>
       </c>
       <c r="D63" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
         <v>58</v>
       </c>
-      <c r="C64">
-        <v>1315</v>
+      <c r="C64" s="4">
+        <v>1276</v>
       </c>
       <c r="D64" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
         <v>59</v>
       </c>
-      <c r="C65">
-        <v>1276</v>
+      <c r="C65" s="4">
+        <v>1290</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
-      </c>
-      <c r="C66">
-        <v>1290</v>
+        <v>65</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1250</v>
       </c>
       <c r="D66" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67">
-        <v>1250</v>
+        <v>91</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1274</v>
       </c>
       <c r="D67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68">
-        <v>1274</v>
+        <v>60</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1255</v>
       </c>
       <c r="D68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
         <v>61</v>
       </c>
-      <c r="C69">
-        <v>1255</v>
+      <c r="C69" s="4">
+        <v>1293</v>
       </c>
       <c r="D69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
         <v>62</v>
       </c>
-      <c r="C70">
-        <v>1293</v>
+      <c r="C70" s="4">
+        <v>1256</v>
       </c>
       <c r="D70" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B71" t="s">
         <v>63</v>
       </c>
-      <c r="C71">
-        <v>1256</v>
+      <c r="C71" s="4">
+        <v>1297</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72">
-        <v>1297</v>
+        <v>63</v>
+      </c>
+      <c r="C72" s="4">
+        <v>1220</v>
       </c>
       <c r="D72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
         <v>64</v>
       </c>
-      <c r="C73">
-        <v>1220</v>
+      <c r="C73" s="4">
+        <v>1280</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>65</v>
-      </c>
-      <c r="C74">
-        <v>1280</v>
+        <v>66</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1281</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
-      </c>
-      <c r="C75">
-        <v>1281</v>
+        <v>94</v>
+      </c>
+      <c r="C75" s="4">
+        <v>1254</v>
       </c>
       <c r="D75" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
-      </c>
-      <c r="C76">
-        <v>1254</v>
+        <v>67</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1253</v>
       </c>
       <c r="D76" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" t="s">
         <v>68</v>
       </c>
-      <c r="C77">
-        <v>1253</v>
+      <c r="C77" s="4">
+        <v>1272</v>
       </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78">
-        <v>1272</v>
+        <v>70</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1222</v>
       </c>
       <c r="D78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
         <v>71</v>
       </c>
-      <c r="C79">
-        <v>1222</v>
+      <c r="C79" s="4">
+        <v>1296</v>
       </c>
       <c r="D79" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
         <v>72</v>
       </c>
-      <c r="C80">
-        <v>1296</v>
+      <c r="C80" s="4">
+        <v>1251</v>
       </c>
       <c r="D80" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
         <v>73</v>
       </c>
-      <c r="C81">
-        <v>1251</v>
+      <c r="C81" s="4">
+        <v>1235</v>
       </c>
       <c r="D81" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B82" t="s">
         <v>74</v>
       </c>
-      <c r="C82">
-        <v>1235</v>
+      <c r="C82" s="4">
+        <v>1204</v>
       </c>
       <c r="D82" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B83" t="s">
-        <v>75</v>
-      </c>
-      <c r="C83">
-        <v>1204</v>
+        <v>21</v>
+      </c>
+      <c r="C83" s="4">
+        <v>1202</v>
       </c>
       <c r="D83" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84">
-        <v>1202</v>
+        <v>75</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1261</v>
       </c>
       <c r="D84" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" t="s">
         <v>76</v>
       </c>
-      <c r="C85">
-        <v>1261</v>
+      <c r="C85" s="4">
+        <v>1310</v>
       </c>
       <c r="D85" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B86" t="s">
         <v>77</v>
       </c>
-      <c r="C86">
-        <v>1310</v>
+      <c r="C86" s="4">
+        <v>1294</v>
       </c>
       <c r="D86" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B87" t="s">
         <v>78</v>
       </c>
-      <c r="C87">
-        <v>1294</v>
+      <c r="C87" s="4">
+        <v>1298</v>
       </c>
       <c r="D87" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88" t="s">
         <v>79</v>
       </c>
-      <c r="C88">
-        <v>1298</v>
+      <c r="C88" s="4">
+        <v>1246</v>
       </c>
       <c r="D88" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B89" t="s">
         <v>80</v>
       </c>
-      <c r="C89">
-        <v>1246</v>
+      <c r="C89" s="4">
+        <v>1221</v>
       </c>
       <c r="D89" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90">
-        <v>1221</v>
+        <v>187</v>
+      </c>
+      <c r="C90" s="4">
+        <v>1266</v>
       </c>
       <c r="D90" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
-      </c>
-      <c r="C91">
-        <v>1266</v>
+        <v>81</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1207</v>
       </c>
       <c r="D91" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="B92" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92">
-        <v>1207</v>
+        <v>195</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1262</v>
       </c>
       <c r="D92" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B93" t="s">
-        <v>197</v>
-      </c>
-      <c r="C93">
-        <v>1262</v>
+        <v>82</v>
+      </c>
+      <c r="C93" s="4">
+        <v>1288</v>
       </c>
       <c r="D93" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
         <v>83</v>
       </c>
-      <c r="C94">
-        <v>1288</v>
+      <c r="C94" s="4">
+        <v>1258</v>
       </c>
       <c r="D94" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B95" t="s">
         <v>84</v>
       </c>
-      <c r="C95">
-        <v>1258</v>
+      <c r="C95" s="4">
+        <v>1203</v>
       </c>
       <c r="D95" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
         <v>85</v>
       </c>
-      <c r="C96">
-        <v>1203</v>
+      <c r="C96" s="4">
+        <v>1316</v>
       </c>
       <c r="D96" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B97" t="s">
-        <v>86</v>
-      </c>
-      <c r="C97">
-        <v>1316</v>
+        <v>96</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1257</v>
       </c>
       <c r="D97" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
-      </c>
-      <c r="C98">
-        <v>1257</v>
+        <v>86</v>
+      </c>
+      <c r="C98" s="4">
+        <v>1292</v>
       </c>
       <c r="D98" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>188</v>
-      </c>
-      <c r="B99" t="s">
-        <v>87</v>
-      </c>
-      <c r="C99">
-        <v>1292</v>
-      </c>
-      <c r="D99" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F93" xr:uid="{83F26A8D-2BE1-46D0-B50A-D1A32A51E35C}">
-    <sortState ref="A2:C99">
-      <sortCondition ref="A1:A99"/>
+  <autoFilter ref="A1:F92" xr:uid="{83F26A8D-2BE1-46D0-B50A-D1A32A51E35C}">
+    <sortState ref="A2:C98">
+      <sortCondition ref="A1:A98"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:CF129">
-    <sortCondition ref="A2:A129"/>
+  <sortState ref="A2:CF128">
+    <sortCondition ref="A2:A128"/>
   </sortState>
-  <conditionalFormatting sqref="C100:C1048576 C1">
-    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
+  <conditionalFormatting sqref="C99:C1048576 C1">
+    <cfRule type="duplicateValues" dxfId="3" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="adriana@2s.com.br&gt;" xr:uid="{AE487F2D-FB0F-0041-8223-8D8916570E82}"/>
+    <hyperlink ref="B26" r:id="rId2" xr:uid="{CEC42E02-123F-0B4F-AFDB-E96DCF466971}"/>
+    <hyperlink ref="B51" r:id="rId3" xr:uid="{B9C36569-A250-BF4E-AFBA-04A7C2892D69}"/>
+    <hyperlink ref="B67" r:id="rId4" xr:uid="{96871D54-05AD-0B45-B134-676BCEE04FC6}"/>
+    <hyperlink ref="B63" r:id="rId5" xr:uid="{3DAD02CF-0FCD-9448-8FED-A919486B8C35}"/>
+    <hyperlink ref="B65" r:id="rId6" xr:uid="{48EE9585-47E2-734D-9773-B4770E76DC3B}"/>
+    <hyperlink ref="B81" r:id="rId7" display="rafael.nunes@2s.com.br&gt;" xr:uid="{E16669AA-56AE-DF48-8BD6-63D763F7262D}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91000523-64C0-CF40-9C79-62A29F96294C}">
+  <dimension ref="A1:D79"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" t="s">
+        <v>452</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" t="s">
+        <v>450</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" t="s">
+        <v>388</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>332</v>
+      </c>
+      <c r="B15" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B17" t="s">
+        <v>389</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B18" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>384</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" t="s">
+        <v>366</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>367</v>
+      </c>
+      <c r="B21" t="s">
+        <v>372</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>306</v>
+      </c>
+      <c r="B22" t="s">
+        <v>385</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" t="s">
+        <v>390</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" t="s">
+        <v>351</v>
+      </c>
+      <c r="C24" t="s">
+        <v>413</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>312</v>
+      </c>
+      <c r="B25" t="s">
+        <v>391</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" t="s">
+        <v>373</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>256</v>
+      </c>
+      <c r="B27" t="s">
+        <v>264</v>
+      </c>
+      <c r="C27" t="s">
+        <v>441</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>313</v>
+      </c>
+      <c r="B28" t="s">
+        <v>392</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>282</v>
+      </c>
+      <c r="B29" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" t="s">
+        <v>418</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>314</v>
+      </c>
+      <c r="B30" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31" t="s">
+        <v>336</v>
+      </c>
+      <c r="C31" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>283</v>
+      </c>
+      <c r="B32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C32" t="s">
+        <v>419</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" t="s">
+        <v>354</v>
+      </c>
+      <c r="C33" t="s">
+        <v>453</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>369</v>
+      </c>
+      <c r="B34" t="s">
+        <v>374</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>315</v>
+      </c>
+      <c r="B35" t="s">
+        <v>394</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>285</v>
+      </c>
+      <c r="B36" t="s">
+        <v>355</v>
+      </c>
+      <c r="C36" t="s">
+        <v>433</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" t="s">
+        <v>356</v>
+      </c>
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>287</v>
+      </c>
+      <c r="B38" t="s">
+        <v>436</v>
+      </c>
+      <c r="C38" t="s">
+        <v>454</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>242</v>
+      </c>
+      <c r="B39" t="s">
+        <v>257</v>
+      </c>
+      <c r="C39" t="s">
+        <v>442</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>316</v>
+      </c>
+      <c r="B41" t="s">
+        <v>395</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>244</v>
+      </c>
+      <c r="B42" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" t="s">
+        <v>443</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>368</v>
+      </c>
+      <c r="B43" t="s">
+        <v>375</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>317</v>
+      </c>
+      <c r="B44" t="s">
+        <v>396</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45" t="s">
+        <v>263</v>
+      </c>
+      <c r="C45" t="s">
+        <v>445</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>288</v>
+      </c>
+      <c r="B46" t="s">
+        <v>357</v>
+      </c>
+      <c r="C46" t="s">
+        <v>455</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>245</v>
+      </c>
+      <c r="B47" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" t="s">
+        <v>265</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>415</v>
+      </c>
+      <c r="B48" t="s">
+        <v>416</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>330</v>
+      </c>
+      <c r="B49" t="s">
+        <v>410</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>299</v>
+      </c>
+      <c r="B50" t="s">
+        <v>376</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>252</v>
+      </c>
+      <c r="B51" t="s">
+        <v>260</v>
+      </c>
+      <c r="C51" t="s">
+        <v>267</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" t="s">
+        <v>345</v>
+      </c>
+      <c r="C52" t="s">
+        <v>447</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>289</v>
+      </c>
+      <c r="B53" t="s">
+        <v>358</v>
+      </c>
+      <c r="C53" t="s">
+        <v>456</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>254</v>
+      </c>
+      <c r="B54" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" t="s">
+        <v>444</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" t="s">
+        <v>397</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>302</v>
+      </c>
+      <c r="B56" t="s">
+        <v>381</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>378</v>
+      </c>
+      <c r="B57" t="s">
+        <v>377</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>290</v>
+      </c>
+      <c r="B58" t="s">
+        <v>359</v>
+      </c>
+      <c r="C58" t="s">
+        <v>422</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>307</v>
+      </c>
+      <c r="B59" t="s">
+        <v>386</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>291</v>
+      </c>
+      <c r="B60" t="s">
+        <v>360</v>
+      </c>
+      <c r="C60" t="s">
+        <v>457</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>327</v>
+      </c>
+      <c r="B61" t="s">
+        <v>407</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>279</v>
+      </c>
+      <c r="B62" t="s">
+        <v>349</v>
+      </c>
+      <c r="C62" t="s">
+        <v>451</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>292</v>
+      </c>
+      <c r="B63" t="s">
+        <v>361</v>
+      </c>
+      <c r="C63" t="s">
+        <v>240</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>319</v>
+      </c>
+      <c r="B64" t="s">
+        <v>398</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>331</v>
+      </c>
+      <c r="B65" t="s">
+        <v>411</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>329</v>
+      </c>
+      <c r="B66" t="s">
+        <v>409</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67" t="s">
+        <v>399</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>293</v>
+      </c>
+      <c r="B68" t="s">
+        <v>362</v>
+      </c>
+      <c r="C68" t="s">
+        <v>458</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>277</v>
+      </c>
+      <c r="B69" t="s">
+        <v>347</v>
+      </c>
+      <c r="C69" t="s">
+        <v>449</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>321</v>
+      </c>
+      <c r="B70" t="s">
+        <v>400</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>322</v>
+      </c>
+      <c r="B71" t="s">
+        <v>401</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>323</v>
+      </c>
+      <c r="B72" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>253</v>
+      </c>
+      <c r="B73" t="s">
+        <v>261</v>
+      </c>
+      <c r="C73" t="s">
+        <v>270</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>300</v>
+      </c>
+      <c r="B74" t="s">
+        <v>379</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>324</v>
+      </c>
+      <c r="B75" t="s">
+        <v>403</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>325</v>
+      </c>
+      <c r="B76" t="s">
+        <v>404</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>333</v>
+      </c>
+      <c r="B77" t="s">
+        <v>406</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>326</v>
+      </c>
+      <c r="B78" t="s">
+        <v>405</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>301</v>
+      </c>
+      <c r="B79" t="s">
+        <v>380</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>521</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D79" xr:uid="{8F5917A4-8758-594C-8C77-C6F1476CB4A2}">
+    <sortState ref="A2:D79">
+      <sortCondition ref="A1:A79"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="C1">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="adriana@2s.com.br&gt;" xr:uid="{AE487F2D-FB0F-0041-8223-8D8916570E82}"/>
-    <hyperlink ref="B26" r:id="rId2" xr:uid="{CEC42E02-123F-0B4F-AFDB-E96DCF466971}"/>
-    <hyperlink ref="B51" r:id="rId3" xr:uid="{B9C36569-A250-BF4E-AFBA-04A7C2892D69}"/>
-    <hyperlink ref="B68" r:id="rId4" xr:uid="{96871D54-05AD-0B45-B134-676BCEE04FC6}"/>
-    <hyperlink ref="B64" r:id="rId5" xr:uid="{3DAD02CF-0FCD-9448-8FED-A919486B8C35}"/>
-    <hyperlink ref="B66" r:id="rId6" xr:uid="{48EE9585-47E2-734D-9773-B4770E76DC3B}"/>
-    <hyperlink ref="B82" r:id="rId7" display="rafael.nunes@2s.com.br&gt;" xr:uid="{E16669AA-56AE-DF48-8BD6-63D763F7262D}"/>
+    <hyperlink ref="B8" r:id="rId1" display="mailto:bzatyrko@cisco.com" xr:uid="{300C3D1C-385D-A049-A673-0D0CA6279181}"/>
+    <hyperlink ref="B40" r:id="rId2" display="mailto:jsardinh@cisco.com" xr:uid="{949FF3D8-FDEF-3542-B306-309D21E88F9D}"/>
+    <hyperlink ref="A14" r:id="rId3" display="http://wwwin-tools.cisco.com/dir/reports/droque" xr:uid="{08578761-45B5-824D-B6AA-99D12A9D0D87}"/>
+    <hyperlink ref="A50" r:id="rId4" display="http://wwwin-tools.cisco.com/dir/reports/lcristov" xr:uid="{D298C7B2-7955-8943-9631-E16036D4BE28}"/>
+    <hyperlink ref="B2" r:id="rId5" display="mailto:aandreol@cisco.com" xr:uid="{A3F0D601-C136-4F4C-BE28-1CCA4003E69A}"/>
+    <hyperlink ref="B31" r:id="rId6" display="mailto:fpratell@cisco.com" xr:uid="{9391C853-2B28-4B4C-860D-9E44051AD394}"/>
+    <hyperlink ref="B7" r:id="rId7" display="mailto:amincovs@cisco.com" xr:uid="{5EC679CC-00FF-4740-8E9B-957C8A306044}"/>
+    <hyperlink ref="B38" r:id="rId8" xr:uid="{A87DBBFB-723A-CC44-88E2-49CD643FCB49}"/>
+    <hyperlink ref="B68" r:id="rId9" xr:uid="{0DC15ABF-4085-E141-AB1B-1E3D9F047142}"/>
+    <hyperlink ref="B63" r:id="rId10" xr:uid="{F31EC07F-5625-C345-B870-F12A3BE6C8CF}"/>
+    <hyperlink ref="B60" r:id="rId11" xr:uid="{777E7F43-838E-F94A-B47C-BC4BCF52688A}"/>
+    <hyperlink ref="B59" r:id="rId12" xr:uid="{083E2ECF-CA82-184B-9C0B-318D30B4EBC4}"/>
+    <hyperlink ref="B55" r:id="rId13" xr:uid="{66A76503-BC34-8040-A6AC-19470F517532}"/>
+    <hyperlink ref="B78" r:id="rId14" xr:uid="{AAF84923-7325-0946-B01D-22780BA9FA02}"/>
+    <hyperlink ref="B61" r:id="rId15" xr:uid="{A563A02E-3DF9-A746-9529-6E3D3AEE206D}"/>
+    <hyperlink ref="B6" r:id="rId16" xr:uid="{5E080B15-A6F0-2049-A8A2-832D0081ADB3}"/>
+    <hyperlink ref="B66" r:id="rId17" xr:uid="{764334A8-C2AF-3048-BF0F-FEAA78BF588B}"/>
+    <hyperlink ref="B49" r:id="rId18" xr:uid="{1761ECA7-BDAA-5540-BC0F-6B15F0B1C1D0}"/>
+    <hyperlink ref="B65" r:id="rId19" xr:uid="{ECA0F33E-DF0D-5142-B885-1ECB2ADAB14C}"/>
+    <hyperlink ref="B15" r:id="rId20" xr:uid="{4CA1E10B-2577-3C4B-8C70-8A6C246CF882}"/>
+    <hyperlink ref="B48" r:id="rId21" display="mailto:lucorrea@cisco.com" xr:uid="{81479879-498E-7742-8278-4025208E5139}"/>
+    <hyperlink ref="C39" r:id="rId22" display="tel:+551155086318" xr:uid="{5CA31CE9-B93F-8E45-9FAE-1EB1A1EA44FB}"/>
+    <hyperlink ref="C42" r:id="rId23" display="tel:+551155086334" xr:uid="{F02FEE2B-A1BE-7145-A390-3D35713C6194}"/>
+    <hyperlink ref="C54" r:id="rId24" display="tel:+551155089968" xr:uid="{8C25901A-E954-A54F-B2D6-79E3672DCA2D}"/>
+    <hyperlink ref="C5" r:id="rId25" display="tel:+551155023111" xr:uid="{BD9068B3-E73D-A146-8F16-8B3F96C3BAA5}"/>
+    <hyperlink ref="C52" r:id="rId26" display="tel:+551155082434" xr:uid="{2A3C1E90-F12E-4943-9F5E-6AC6F6BC4B38}"/>
+    <hyperlink ref="C12" r:id="rId27" display="tel:+552124836353" xr:uid="{F1335AD7-D30B-7046-BB26-855FA3050F94}"/>
+    <hyperlink ref="C69" r:id="rId28" display="tel:+552124837275" xr:uid="{073AFC2E-B804-AF4A-853E-8D20B0E10BF0}"/>
+    <hyperlink ref="C10" r:id="rId29" display="tel:+551126669111" xr:uid="{EF27CFD5-3122-8943-A1A0-A39895274A90}"/>
+    <hyperlink ref="C62" r:id="rId30" display="tel:+551155023196" xr:uid="{F723123D-36DB-5045-BFD2-C900108B5B46}"/>
+    <hyperlink ref="C9" r:id="rId31" display="tel:+551155082489" xr:uid="{322B78B2-AB28-C243-B041-D37106F0D7E8}"/>
+    <hyperlink ref="C33" r:id="rId32" display="tel:+551155081534" xr:uid="{245472C3-E384-D447-89EB-48E6006C436E}"/>
+    <hyperlink ref="C60" r:id="rId33" display="tel:+551126669248" xr:uid="{D6093DD9-7E26-3942-A8EA-218B79E22284}"/>
+    <hyperlink ref="C68" r:id="rId34" display="tel:+551126669148" xr:uid="{77A4F173-B6B0-0643-9302-781484BF3293}"/>
+    <hyperlink ref="C11" r:id="rId35" display="tel:+552176299426" xr:uid="{CE24BAF3-EFEC-6C4F-B9F8-3DB283D8959C}"/>
+    <hyperlink ref="C14" r:id="rId36" display="tel:+551155023113" xr:uid="{87B17570-FC74-9A47-A44D-013611CC7C49}"/>
+    <hyperlink ref="C20" r:id="rId37" display="tel:+551155081576" xr:uid="{5A9AC4EB-4CDB-1644-8710-929176FF863C}"/>
+    <hyperlink ref="C34" r:id="rId38" display="tel:+552124836310" xr:uid="{1EEDF4A8-C378-BA42-BB31-AE851B0D3ACD}"/>
+    <hyperlink ref="C43" r:id="rId39" display="tel:+551155023178" xr:uid="{0E60A07C-6210-E642-879B-B2840E05582C}"/>
+    <hyperlink ref="C50" r:id="rId40" display="tel:+551155081589" xr:uid="{18EAF337-E8A4-D449-B6ED-653599059C6E}"/>
+    <hyperlink ref="C57" r:id="rId41" display="tel:+551155023122" xr:uid="{68BF0A30-76A5-F94E-909C-969C3001957C}"/>
+    <hyperlink ref="C79" r:id="rId42" display="tel:+551155081579" xr:uid="{1E64D796-913D-2E46-98C0-AB82CABD9C80}"/>
+    <hyperlink ref="C56" r:id="rId43" display="tel:+551155023197" xr:uid="{E2037197-E7CA-A644-BF51-681FCBE142C4}"/>
+    <hyperlink ref="C3" r:id="rId44" display="tel:+551155089922" xr:uid="{D95C8183-96D7-1242-9C71-44D4E8B4959E}"/>
+    <hyperlink ref="C18" r:id="rId45" display="tel:+551155089906" xr:uid="{B720B70A-474D-A54D-8517-A85A6FA8C96D}"/>
+    <hyperlink ref="C19" r:id="rId46" display="tel:+551155086329" xr:uid="{A6C033F8-E096-A04B-889B-442DCB0A7159}"/>
+    <hyperlink ref="C22" r:id="rId47" display="tel:+551155086338" xr:uid="{0901CF91-D399-DF46-9029-3827271BCCF5}"/>
+    <hyperlink ref="C59" r:id="rId48" display="tel:+552124836308" xr:uid="{666C21D1-DC4B-5A4C-B1DA-332E3C5F7070}"/>
+    <hyperlink ref="C13" r:id="rId49" display="tel:+551155089986" xr:uid="{597ADD01-F055-8D42-AA96-AEEC66EACC36}"/>
+    <hyperlink ref="C17" r:id="rId50" display="tel:+552124836390" xr:uid="{A9062BDE-AD1F-E040-B4D5-049AA664D913}"/>
+    <hyperlink ref="C23" r:id="rId51" display="tel:+551155089995" xr:uid="{C6A7F2D8-B2F9-0345-BDC0-340DD4A7E905}"/>
+    <hyperlink ref="C28" r:id="rId52" display="tel:+551126669316" xr:uid="{286855A5-4321-1D4B-BBAC-6F2357306212}"/>
+    <hyperlink ref="C30" r:id="rId53" display="tel:+551155082469" xr:uid="{74E7C43A-8F63-F64B-A236-A280AEECB73E}"/>
+    <hyperlink ref="C35" r:id="rId54" display="tel:+551155082412" xr:uid="{4924B3BB-F9FF-AD40-ABC5-B58951081950}"/>
+    <hyperlink ref="C41" r:id="rId55" display="tel:+551155086312" xr:uid="{8985CEB9-9AC0-1D44-96B7-49956C3A50E7}"/>
+    <hyperlink ref="C44" r:id="rId56" display="tel:+551155082456" xr:uid="{CAA7BD0D-E529-B641-8871-25F87591E396}"/>
+    <hyperlink ref="C55" r:id="rId57" display="tel:+551126669293" xr:uid="{7B28350F-C6F1-C040-9008-75A82EE677E5}"/>
+    <hyperlink ref="C67" r:id="rId58" display="tel:+551155082420" xr:uid="{0C30D5B0-246D-B141-BB90-E3B56EC67A50}"/>
+    <hyperlink ref="C70" r:id="rId59" display="tel:+14088953828" xr:uid="{CF0AB937-BA7D-D647-9EB5-817683430B16}"/>
+    <hyperlink ref="C71" r:id="rId60" display="tel:+551155089928" xr:uid="{2BBB24D4-6F62-7542-B908-A6D174187F73}"/>
+    <hyperlink ref="C78" r:id="rId61" display="tel:+551155081570" xr:uid="{E79D28E5-7498-AB43-AF64-9B4CE651CBE3}"/>
+    <hyperlink ref="C76" r:id="rId62" display="tel:+551155082495" xr:uid="{48B42802-DD2F-EA4E-894A-E0D99F6BD5F3}"/>
+    <hyperlink ref="C75" r:id="rId63" display="tel:+551155023193" xr:uid="{D07082CC-C5B5-7F4D-B063-733F39FEA5FC}"/>
+    <hyperlink ref="C72" r:id="rId64" display="tel:+551155086316" xr:uid="{047F2A96-EC59-D541-A554-BBD99509CA78}"/>
+    <hyperlink ref="C15" r:id="rId65" display="tel:+551155023166" xr:uid="{DB934CE6-F633-944F-8835-FDB940A9DF8F}"/>
+    <hyperlink ref="C65" r:id="rId66" display="tel:+551155086337" xr:uid="{8DC5A786-3CCE-FB4C-938E-1EC7E5E6B7FD}"/>
+    <hyperlink ref="C49" r:id="rId67" display="tel:+551155089924" xr:uid="{0AD8F16F-409C-9143-8599-58EDE940A5EE}"/>
+    <hyperlink ref="C66" r:id="rId68" display="tel:+551155023184" xr:uid="{A909BA54-B7AA-CA47-A385-D941EA0289A5}"/>
+    <hyperlink ref="C6" r:id="rId69" display="tel:+551155086345" xr:uid="{4A1BE2E8-54BC-B94B-98DA-5E49A1C17C61}"/>
+    <hyperlink ref="C61" r:id="rId70" display="tel:+551155082457" xr:uid="{D4FCBA48-E360-994D-A0E2-7BF3CAD9C302}"/>
+    <hyperlink ref="D15" r:id="rId71" display="tel:+5511942874780" xr:uid="{D0DC928A-7A99-7C4E-947F-2C55811145A4}"/>
+    <hyperlink ref="D65" r:id="rId72" display="tel:+5511992513510" xr:uid="{EF4A4F0D-301B-5941-8BDE-73B283F08FD3}"/>
+    <hyperlink ref="D49" r:id="rId73" display="tel:+5511992305378" xr:uid="{1B9FC2C1-191E-CF49-B323-0C25DBE7DFBB}"/>
+    <hyperlink ref="D66" r:id="rId74" display="tel:+5511992605331" xr:uid="{89B066FF-9DA7-F240-8053-9FDC0890C95F}"/>
+    <hyperlink ref="D6" r:id="rId75" display="tel:+5511992513297" xr:uid="{A105AD22-35B7-8B48-8A69-48259BFD3CEF}"/>
+    <hyperlink ref="D61" r:id="rId76" display="tel:+5511976345431" xr:uid="{4CEE3CA5-3C0F-FB42-A60C-DA4FBFAC3AA0}"/>
+    <hyperlink ref="D41" r:id="rId77" display="tel:+5511992513124" xr:uid="{C8D93588-8963-F643-B5D1-CB1E7BE3B504}"/>
+    <hyperlink ref="D44" r:id="rId78" display="tel:+5511992516750" xr:uid="{921263EB-EB19-F54D-80AE-4F2E1D3E0F29}"/>
+    <hyperlink ref="D55" r:id="rId79" display="tel:+5511992505937" xr:uid="{35A50C2B-BC57-2C47-93DC-E8F14DAE4EAE}"/>
+    <hyperlink ref="D64" r:id="rId80" display="tel:+551192514718" xr:uid="{D9B9EA02-51E7-F24E-B2B5-47223ACAE15B}"/>
+    <hyperlink ref="D67" r:id="rId81" display="tel:+5511992517614" xr:uid="{C519701A-1FD7-B843-9BBE-310568823955}"/>
+    <hyperlink ref="D71" r:id="rId82" display="tel:+5511992507147" xr:uid="{A8789A02-D1E8-CB49-8D10-5C145D8FA617}"/>
+    <hyperlink ref="D77" r:id="rId83" display="tel:+5511992511472" xr:uid="{044DD5B6-ECA3-A346-8E19-DBE4F2ECB3AE}"/>
+    <hyperlink ref="D78" r:id="rId84" display="tel:+5511982330042" xr:uid="{D0814B8C-8A3C-384F-A35A-CFD69E224887}"/>
+    <hyperlink ref="D76" r:id="rId85" display="tel:+5511992511236" xr:uid="{15A72105-0CD0-E44F-8D08-D083CB5B8186}"/>
+    <hyperlink ref="D75" r:id="rId86" display="tel:+5511941340606" xr:uid="{601EBD72-ECB8-C743-AAC0-AD43DFB86BBB}"/>
+    <hyperlink ref="D72" r:id="rId87" display="tel:+5511976594093" xr:uid="{C8794860-0E73-B647-A1C5-71160912542B}"/>
+    <hyperlink ref="D28" r:id="rId88" display="tel:+5511991341196" xr:uid="{A2082A03-BBCA-B244-A775-9D7FECB93542}"/>
+    <hyperlink ref="D17" r:id="rId89" display="tel:+5521986047649" xr:uid="{D643D0BF-4406-D74E-8BD0-2798356A88D3}"/>
+    <hyperlink ref="D59" r:id="rId90" display="tel:+552176295643" xr:uid="{1693DE3A-E6A3-514A-9044-8FA55C76E51D}"/>
+    <hyperlink ref="D13" r:id="rId91" display="tel:+5511992515244" xr:uid="{1D2AC06E-6F1D-2948-9869-23EF986064A2}"/>
+    <hyperlink ref="D79" r:id="rId92" display="tel:+5511992513808" xr:uid="{C62726D6-D80C-0F4D-A45D-2326298C32F2}"/>
+    <hyperlink ref="D3" r:id="rId93" display="tel:+5511950381278" xr:uid="{BEA17BA2-CC27-6F49-A6E9-5B3DA10CCC08}"/>
+    <hyperlink ref="D18" r:id="rId94" display="tel:+5511992529912" xr:uid="{DB73F3E5-889F-2847-8E89-F112A9BBDFE9}"/>
+    <hyperlink ref="D19" r:id="rId95" display="tel:+5511992523426" xr:uid="{E2237579-F56D-084F-9153-CA8BFE27904C}"/>
+    <hyperlink ref="D22" r:id="rId96" display="tel:+5511992540090" xr:uid="{98F5EEF7-2EE6-CF48-A839-A9F6894EE734}"/>
+    <hyperlink ref="D43" r:id="rId97" display="tel:+5511992517465" xr:uid="{67A8BA54-A910-E24A-AEC8-CA96F16B1C65}"/>
+    <hyperlink ref="D14" r:id="rId98" display="tel:+5511992512191" xr:uid="{D0001961-99A0-024F-8387-54C8606DCDD1}"/>
+    <hyperlink ref="D16" r:id="rId99" display="tel:+5511992518527" xr:uid="{BDD745AD-270C-6D49-9FF4-BBC166E1EEDE}"/>
+    <hyperlink ref="D20" r:id="rId100" display="tel:+5511992515533" xr:uid="{60C6B0DE-A9AE-E24C-90C1-D319FB3B8ACA}"/>
+    <hyperlink ref="D34" r:id="rId101" display="tel:+5521976295502" xr:uid="{0DABF5D2-8A53-5F44-99D4-71F080E952C9}"/>
+    <hyperlink ref="D33" r:id="rId102" display="tel:+5511992517967" xr:uid="{B46097B9-E016-A346-992F-AE6FA1F7DEC0}"/>
+    <hyperlink ref="D60" r:id="rId103" display="tel:+5561996441759" xr:uid="{ACD22789-16D9-0C43-8354-889F43E6E40B}"/>
+    <hyperlink ref="D68" r:id="rId104" display="tel:+5511961765969" xr:uid="{05D9D6ED-256E-5C48-BB91-975395AC9C12}"/>
+    <hyperlink ref="D9" r:id="rId105" display="tel:+5551997618484" xr:uid="{66ABD3CC-55E9-6740-B35C-221C29954762}"/>
+    <hyperlink ref="D39" r:id="rId106" display="tel:+5511992517612" xr:uid="{9ECFD2DE-D615-914C-8C13-6FF3B4D37CB1}"/>
+    <hyperlink ref="D42" r:id="rId107" display="tel:+5511981405000" xr:uid="{CB99587D-B746-734F-A297-D82531D89843}"/>
+    <hyperlink ref="D54" r:id="rId108" display="tel:+5511992511276" xr:uid="{EA50F50B-1B14-E849-90B9-2FA233364392}"/>
+    <hyperlink ref="D69" r:id="rId109" display="tel:+5521976295713" xr:uid="{71DA939C-2F48-3543-9909-D57C3C3C5B61}"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>